<commit_message>
Q42 trapped water solved
</commit_message>
<xml_diff>
--- a/Leetcode_150_challenge.xlsx
+++ b/Leetcode_150_challenge.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Leetcode_150_Challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502506A7-139A-42B9-A70F-16275666A00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD5D19B-D2C9-449A-A405-291C2EB0B83C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{EB447855-6AA0-463B-8026-A1186D00A3CE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>Problem</t>
   </si>
@@ -175,12 +175,37 @@
   <si>
     <t>Think of it as pivot. Get products starting from 1 to right. Then take thaat array in for loop again and multiply with reverse products.</t>
   </si>
+  <si>
+    <t>Since majority element will be always present n/2 times, just sort the array and return n/2th element.</t>
+  </si>
+  <si>
+    <t>Trapping rain water</t>
+  </si>
+  <si>
+    <t>Hard</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">to calculate trapped water, limiting height is left side. Calculate max left, max right arrays for every I position and use </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Min(MaxL,MaxR) - H[i] and add it to calculate trapped water.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +235,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -217,12 +264,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -238,7 +279,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -270,59 +317,64 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFD00000"/>
+      <color rgb="FFE04040"/>
+      <color rgb="FFE06666"/>
+      <color rgb="FFCD2929"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -633,248 +685,258 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131AB193-7762-4DE5-B735-45D330CD43B8}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="C9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6.90625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="42" customWidth="1"/>
-    <col min="3" max="3" width="10.26953125" customWidth="1"/>
+    <col min="2" max="2" width="39.453125" customWidth="1"/>
+    <col min="3" max="3" width="11.08984375" customWidth="1"/>
     <col min="4" max="4" width="169.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="15" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="10">
+      <c r="A3" s="2">
         <v>88</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="33.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="13">
+      <c r="A4" s="2">
         <v>27</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="13">
+      <c r="A5" s="2">
         <v>26</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="68.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="13">
+      <c r="A6" s="2">
         <v>80</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="18">
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="11">
         <v>169</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="17"/>
+      <c r="D7" s="12" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="91.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="13">
+      <c r="A8" s="2">
         <v>189</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="54.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="13">
+      <c r="A9" s="2">
         <v>121</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="13">
+      <c r="A10" s="2">
         <v>122</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="13">
+      <c r="A11" s="2">
         <v>238</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="13">
+      <c r="A12" s="2">
         <v>134</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
+    <row r="13" spans="1:4" ht="29.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="3">
+        <v>42</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="13"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="13"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="13"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="13"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="13"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
+      <c r="A22" s="3"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="13"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
+      <c r="A23" s="3"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="13"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
+      <c r="A24" s="3"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="13"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
+      <c r="A25" s="3"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added description in excel
</commit_message>
<xml_diff>
--- a/Leetcode_150_challenge.xlsx
+++ b/Leetcode_150_challenge.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Leetcode_150_Challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761F2A0C-889A-4A8B-B2A7-E45408A3A1A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00071566-9F97-4B8A-A458-61CAB9C422F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{EB447855-6AA0-463B-8026-A1186D00A3CE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t>Problem</t>
   </si>
@@ -486,6 +486,13 @@
   </si>
   <si>
     <t>Is Subsequence</t>
+  </si>
+  <si>
+    <t>1. Used the approach for 2 pointer.
+2. Initialize two pointers i and j. These go from 0 -&gt; s.size() - 1 and t.size() -1 respectively.
+3. The goal is to increase pointer for s only when char matches so that the next char can be searched. The pointer for t(or the striong in which we are searching) increases everytime, hence it is the fast pointer.
+4. if the string matches then increase s pointer i.e. i. 
+5. If the i reaches to s.size() then return true. Return false by default.</t>
   </si>
 </sst>
 </file>
@@ -1000,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131AB193-7762-4DE5-B735-45D330CD43B8}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1265,7 +1272,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="88.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="2">
         <v>392</v>
       </c>
@@ -1275,7 +1282,9 @@
       <c r="C20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3"/>

</xml_diff>